<commit_message>
finalized dataset. ready for eda
</commit_message>
<xml_diff>
--- a/data/league_data/spain/19/spain_defending.xlsx
+++ b/data/league_data/spain/19/spain_defending.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjitvarma/Desktop/trial_git/Predicting-Football-Player-Transfer-Values/data/league_data/spain/19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCED119-C0DA-0E41-98E0-F757AC2CBCCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E89F718-A556-AC4B-B54A-4AD339B041D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1615,9 +1615,6 @@
     <t>Cheick Doukouré</t>
   </si>
   <si>
-    <t>Emerson</t>
-  </si>
-  <si>
     <t>Ignasi Miquel</t>
   </si>
   <si>
@@ -1802,6 +1799,9 @@
   </si>
   <si>
     <t>Juanfran Moreno</t>
+  </si>
+  <si>
+    <t>Emerson Royal</t>
   </si>
 </sst>
 </file>
@@ -2668,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="B259" sqref="B259"/>
+    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
+      <selection activeCell="B437" sqref="B437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13629,7 +13629,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>28</v>
@@ -23794,7 +23794,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>28</v>
@@ -27214,7 +27214,7 @@
         <v>258</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>28</v>
@@ -28542,7 +28542,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>78</v>
@@ -31861,7 +31861,7 @@
         <v>307</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C308" s="3" t="s">
         <v>28</v>
@@ -44088,7 +44088,7 @@
         <v>436</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>531</v>
+        <v>593</v>
       </c>
       <c r="C437" s="3" t="s">
         <v>78</v>
@@ -44183,7 +44183,7 @@
         <v>437</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C438" s="3" t="s">
         <v>28</v>
@@ -44278,7 +44278,7 @@
         <v>438</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C439" s="3" t="s">
         <v>28</v>
@@ -44373,7 +44373,7 @@
         <v>439</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C440" s="3" t="s">
         <v>28</v>
@@ -44468,7 +44468,7 @@
         <v>440</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C441" s="3" t="s">
         <v>28</v>
@@ -44563,7 +44563,7 @@
         <v>441</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C442" s="3" t="s">
         <v>40</v>
@@ -44658,7 +44658,7 @@
         <v>442</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C443" s="3" t="s">
         <v>28</v>
@@ -44753,7 +44753,7 @@
         <v>443</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C444" s="3" t="s">
         <v>47</v>
@@ -44848,7 +44848,7 @@
         <v>444</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C445" s="3" t="s">
         <v>28</v>
@@ -44943,7 +44943,7 @@
         <v>445</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C446" s="3" t="s">
         <v>331</v>
@@ -45034,7 +45034,7 @@
         <v>446</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C447" s="3" t="s">
         <v>28</v>
@@ -45129,7 +45129,7 @@
         <v>447</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C448" s="3" t="s">
         <v>28</v>
@@ -45224,7 +45224,7 @@
         <v>448</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C449" s="3" t="s">
         <v>28</v>
@@ -45315,7 +45315,7 @@
         <v>449</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C450" s="3" t="s">
         <v>28</v>
@@ -45406,7 +45406,7 @@
         <v>450</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C451" s="3" t="s">
         <v>237</v>
@@ -45501,7 +45501,7 @@
         <v>451</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C452" s="3" t="s">
         <v>28</v>
@@ -45596,7 +45596,7 @@
         <v>452</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C453" s="3" t="s">
         <v>269</v>
@@ -45689,7 +45689,7 @@
         <v>453</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C454" s="3" t="s">
         <v>28</v>
@@ -45784,7 +45784,7 @@
         <v>454</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C455" s="3" t="s">
         <v>28</v>
@@ -45879,7 +45879,7 @@
         <v>455</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C456" s="3" t="s">
         <v>198</v>
@@ -45974,7 +45974,7 @@
         <v>456</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C457" s="3" t="s">
         <v>237</v>
@@ -46069,7 +46069,7 @@
         <v>457</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C458" s="3" t="s">
         <v>191</v>
@@ -46164,7 +46164,7 @@
         <v>458</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C459" s="3" t="s">
         <v>78</v>
@@ -46259,7 +46259,7 @@
         <v>459</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C460" s="3" t="s">
         <v>200</v>
@@ -46354,7 +46354,7 @@
         <v>460</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C461" s="3" t="s">
         <v>60</v>
@@ -46449,7 +46449,7 @@
         <v>461</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C462" s="3" t="s">
         <v>40</v>
@@ -46544,7 +46544,7 @@
         <v>462</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C463" s="3" t="s">
         <v>28</v>
@@ -46639,7 +46639,7 @@
         <v>463</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C464" s="3" t="s">
         <v>110</v>
@@ -46734,7 +46734,7 @@
         <v>464</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C465" s="3" t="s">
         <v>28</v>
@@ -46829,7 +46829,7 @@
         <v>465</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C466" s="3" t="s">
         <v>110</v>
@@ -47019,7 +47019,7 @@
         <v>467</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C468" s="3" t="s">
         <v>28</v>
@@ -47114,7 +47114,7 @@
         <v>468</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C469" s="3" t="s">
         <v>28</v>
@@ -47304,7 +47304,7 @@
         <v>470</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C471" s="3" t="s">
         <v>28</v>
@@ -47399,7 +47399,7 @@
         <v>471</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C472" s="3" t="s">
         <v>28</v>
@@ -47494,7 +47494,7 @@
         <v>472</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C473" s="3" t="s">
         <v>28</v>
@@ -47589,7 +47589,7 @@
         <v>473</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C474" s="3" t="s">
         <v>28</v>
@@ -47684,7 +47684,7 @@
         <v>474</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C475" s="3" t="s">
         <v>110</v>
@@ -47779,7 +47779,7 @@
         <v>475</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C476" s="3" t="s">
         <v>237</v>
@@ -47874,7 +47874,7 @@
         <v>476</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C477" s="3" t="s">
         <v>28</v>
@@ -47969,7 +47969,7 @@
         <v>477</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C478" s="3" t="s">
         <v>487</v>
@@ -48064,7 +48064,7 @@
         <v>478</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C479" s="3" t="s">
         <v>28</v>
@@ -48252,7 +48252,7 @@
         <v>480</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C481" s="3" t="s">
         <v>28</v>
@@ -48347,7 +48347,7 @@
         <v>481</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C482" s="3" t="s">
         <v>28</v>
@@ -48442,7 +48442,7 @@
         <v>482</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C483" s="3" t="s">
         <v>47</v>
@@ -48537,7 +48537,7 @@
         <v>483</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C484" s="3" t="s">
         <v>28</v>
@@ -48632,7 +48632,7 @@
         <v>484</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C485" s="3" t="s">
         <v>28</v>
@@ -48727,7 +48727,7 @@
         <v>485</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C486" s="3" t="s">
         <v>136</v>
@@ -48822,7 +48822,7 @@
         <v>486</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C487" s="3" t="s">
         <v>28</v>
@@ -48917,7 +48917,7 @@
         <v>487</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C488" s="3" t="s">
         <v>136</v>
@@ -49012,7 +49012,7 @@
         <v>488</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C489" s="3" t="s">
         <v>28</v>
@@ -49107,7 +49107,7 @@
         <v>489</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C490" s="3" t="s">
         <v>28</v>
@@ -49202,7 +49202,7 @@
         <v>490</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C491" s="3" t="s">
         <v>28</v>
@@ -49297,7 +49297,7 @@
         <v>491</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C492" s="3" t="s">
         <v>28</v>
@@ -49388,7 +49388,7 @@
         <v>492</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C493" s="3" t="s">
         <v>28</v>
@@ -49481,7 +49481,7 @@
         <v>493</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C494" s="3" t="s">
         <v>110</v>
@@ -49572,7 +49572,7 @@
         <v>494</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C495" s="3" t="s">
         <v>28</v>
@@ -49663,7 +49663,7 @@
         <v>495</v>
       </c>
       <c r="B496" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C496" s="3" t="s">
         <v>28</v>
@@ -49758,7 +49758,7 @@
         <v>496</v>
       </c>
       <c r="B497" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C497" s="3" t="s">
         <v>28</v>
@@ -49853,7 +49853,7 @@
         <v>497</v>
       </c>
       <c r="B498" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C498" s="3" t="s">
         <v>172</v>
@@ -49948,7 +49948,7 @@
         <v>498</v>
       </c>
       <c r="B499" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C499" s="3" t="s">
         <v>28</v>
@@ -50043,7 +50043,7 @@
         <v>499</v>
       </c>
       <c r="B500" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C500" s="3" t="s">
         <v>136</v>

</xml_diff>